<commit_message>
updates on ui regression
</commit_message>
<xml_diff>
--- a/websites_links/website_links.xlsx
+++ b/websites_links/website_links.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{68CA39F3-CF75-44F7-B9E7-9BAFFD8C5206}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9385ACB6-D882-4012-8655-7C69A0C22C3E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>baseline_links</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>https://www.kaufmanbroad.fr/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/</t>
   </si>
 </sst>
 </file>
@@ -369,7 +372,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,11 +398,19 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{15D16C3E-1CDF-4FE3-A3E4-A13D415D8B89}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{5168433C-04BD-4B6C-B67D-AA5800BD9DD1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
timeout added for js elements
</commit_message>
<xml_diff>
--- a/websites_links/website_links.xlsx
+++ b/websites_links/website_links.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9385ACB6-D882-4012-8655-7C69A0C22C3E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B3A9CFB7-3B86-45C2-B8C9-0AC834E97C14}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>baseline_links</t>
   </si>
@@ -28,10 +28,7 @@
     <t>test_links</t>
   </si>
   <si>
-    <t>https://www.kaufmanbroad.fr/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/</t>
+    <t>https://www.proximity.mu/</t>
   </si>
 </sst>
 </file>
@@ -372,7 +369,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,19 +395,11 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{15D16C3E-1CDF-4FE3-A3E4-A13D415D8B89}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{5168433C-04BD-4B6C-B67D-AA5800BD9DD1}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>